<commit_message>
Clean up codebase: Remove old files, update gitignore, and improve driver manager
- Removed old/unused files: details_clicker.py, driverslib.py, input_dialog.py, process_data.py, web_input.py
- Added old_codes/ directory to .gitignore
- Updated driver_manager.py with improved error handling
- Updated system_constants.json and other configuration files
- Cleaned up build and dist directories
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -556,10 +556,76 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>3,766</t>
+          <t>5,022</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
+        <is>
+          <t>79,648</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2024-10-25 16:48</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>18,832</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>79,648</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2024-10-10 17:23</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>21,971</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>79,648</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2024-09-30 17:45</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>22,599</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
         <is>
           <t>79,648</t>
         </is>

</xml_diff>

<commit_message>
Implement detailed progress tracking system and clean up interface
- Added real-time progress tracking with current/total counts (3/8 format)
- Implemented progress tracker module for web interface communication
- Added progress endpoints (/progress, /check-status) for real-time updates
- Enhanced Excel data processing with company name as first column
- Implemented append mode for Excel to act as database (no duplicates)
- Removed terminal progress bars for cleaner output
- Fixed premature completion messages timing
- Cleaned up debug messages and overlapping text
- Improved web interface progress display with smart updates
- Added proper error handling and completion signaling
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,20 +436,25 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>회사명</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>발행시간</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>회차</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>추가주식수(주)</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>발행/전환/행사가액(원)</t>
         </is>
@@ -458,20 +463,23 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>에스티팜</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
           <t>2025-09-23 17:00</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
+      <c r="C2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" t="inlineStr">
         <is>
           <t>509,246</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="E2" t="inlineStr">
         <is>
           <t>68,729</t>
         </is>
@@ -480,20 +488,23 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>에스티팜</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
           <t>2025-09-17 17:24</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
+      <c r="C3" t="n">
+        <v>2</v>
+      </c>
+      <c r="D3" t="inlineStr">
         <is>
           <t>35,156</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="E3" t="inlineStr">
         <is>
           <t>79,648</t>
         </is>
@@ -502,20 +513,23 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>에스티팜</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
           <t>2024-12-27 16:49</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
+      <c r="C4" t="n">
+        <v>2</v>
+      </c>
+      <c r="D4" t="inlineStr">
         <is>
           <t>17,578</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="E4" t="inlineStr">
         <is>
           <t>79,648</t>
         </is>
@@ -524,20 +538,23 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
+          <t>에스티팜</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
           <t>2024-12-09 17:23</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
+      <c r="C5" t="n">
+        <v>2</v>
+      </c>
+      <c r="D5" t="inlineStr">
         <is>
           <t>3,766</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="E5" t="inlineStr">
         <is>
           <t>79,648</t>
         </is>
@@ -546,20 +563,23 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
+          <t>에스티팜</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
           <t>2024-11-21 17:13</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
+      <c r="C6" t="n">
+        <v>2</v>
+      </c>
+      <c r="D6" t="inlineStr">
         <is>
           <t>5,022</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="E6" t="inlineStr">
         <is>
           <t>79,648</t>
         </is>
@@ -568,20 +588,23 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
+          <t>에스티팜</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
           <t>2024-10-25 16:48</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
+      <c r="C7" t="n">
+        <v>2</v>
+      </c>
+      <c r="D7" t="inlineStr">
         <is>
           <t>18,832</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="E7" t="inlineStr">
         <is>
           <t>79,648</t>
         </is>
@@ -590,20 +613,23 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
+          <t>에스티팜</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
           <t>2024-10-10 17:23</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
+      <c r="C8" t="n">
+        <v>2</v>
+      </c>
+      <c r="D8" t="inlineStr">
         <is>
           <t>21,971</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="E8" t="inlineStr">
         <is>
           <t>79,648</t>
         </is>
@@ -612,20 +638,23 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
+          <t>에스티팜</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
           <t>2024-09-30 17:45</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
+      <c r="C9" t="n">
+        <v>2</v>
+      </c>
+      <c r="D9" t="inlineStr">
         <is>
           <t>22,599</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="E9" t="inlineStr">
         <is>
           <t>79,648</t>
         </is>

</xml_diff>

<commit_message>
Remove user_settings.json; numeric timing; save coercion; simplify progress UI; drop completed flag; cleanup
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -660,6 +660,356 @@
         </is>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>에스티팜</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>2024-09-12 17:20</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>2</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>43,315</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>79,648</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>에스티팜</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>2024-09-12 17:20</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>2</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>21,971</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>79,648</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>에스티팜</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>2024-09-09 16:50</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>2</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>119,272</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>79,648</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>에스티팜</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>2024-09-04 17:22</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>2</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>17,577</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>79,648</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>에스티팜</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>2024-09-04 17:22</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>2</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>47,709</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>79,648</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>에스티팜</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>2024-09-03 17:23</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>2</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>32,639</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>79,648</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>에스티팜</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>2024-09-02 17:28</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>2</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>50,534</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>79,648</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>에스티팜</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>2024-08-29 16:38</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>2</v>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>4,394</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>79,648</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>에스티팜</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>2024-08-28 16:47</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>2</v>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>43,943</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>79,648</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>에스티팜</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>2024-07-22 17:02</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>1</v>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>218,248</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>68,729</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>에스티팜</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>2024-06-14 16:32</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>1</v>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>145,498</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>68,729</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>에스티팜</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>2024-05-24 17:07</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>1</v>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>181,873</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>68,729</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>에스티팜</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>2024-05-17 16:41</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>1</v>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>202,243</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>68,729</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>에스티팜</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>2024-04-02 17:22</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>1</v>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>125,129</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>68,729</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
UI: two-step flow, records view with round filter, Close flow; Data: JSON saving keeps multiple rows per timestamp; Progress: show total, 100% after processing; Remove completed flag; Settings numeric coercion; Misc fixes
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1010,6 +1010,481 @@
         </is>
       </c>
     </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>한울소재과학</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>2025-10-02 17:05</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>4</v>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>217,013</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>2,304</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>한울소재과학</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>2025-10-02 17:05</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>5</v>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>217,013</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>2,304</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>한울소재과학</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>2025-07-09 16:45</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>5</v>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>173,611</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>2,304</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>한울소재과학</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>2025-07-09 16:45</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>5</v>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>108,506</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>2,304</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>한울소재과학</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>2025-07-01 17:40</t>
+        </is>
+      </c>
+      <c r="C28" t="n">
+        <v>2</v>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>217,013</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>2,304</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>한울소재과학</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>2025-07-01 17:39</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
+        <v>5</v>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>520,832</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>2,304</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>한울소재과학</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>2025-05-28 16:39</t>
+        </is>
+      </c>
+      <c r="C30" t="n">
+        <v>2</v>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>86,805</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>2,304</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>한울소재과학</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>2025-04-23 16:58</t>
+        </is>
+      </c>
+      <c r="C31" t="n">
+        <v>4</v>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>651,039</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>2,304</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>한울소재과학</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>2025-04-23 16:58</t>
+        </is>
+      </c>
+      <c r="C32" t="n">
+        <v>5</v>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>325,519</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>2,304</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>한울소재과학</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>2025-04-16 16:46</t>
+        </is>
+      </c>
+      <c r="C33" t="n">
+        <v>2</v>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>781,245</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>2,304</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>한울소재과학</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>2025-04-16 16:39</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>5</v>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>260,416</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>2,304</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>한울소재과학</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>2025-03-26 17:11</t>
+        </is>
+      </c>
+      <c r="C35" t="n">
+        <v>5</v>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>108,506</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>2,304</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>한울소재과학</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>2025-03-20 17:23</t>
+        </is>
+      </c>
+      <c r="C36" t="n">
+        <v>4</v>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>651,040</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>2,304</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>한울소재과학</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>2025-03-20 17:23</t>
+        </is>
+      </c>
+      <c r="C37" t="n">
+        <v>5</v>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>173,610</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>2,304</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>한울소재과학</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>2025-03-14 17:24</t>
+        </is>
+      </c>
+      <c r="C38" t="n">
+        <v>4</v>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>217,012</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>2,304</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>한울소재과학</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>2025-03-14 17:24</t>
+        </is>
+      </c>
+      <c r="C39" t="n">
+        <v>5</v>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>43,402</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>2,304</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>한울소재과학</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>2025-02-19 17:37</t>
+        </is>
+      </c>
+      <c r="C40" t="n">
+        <v>4</v>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>4,014,741</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>2,304</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>한울소재과학</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>2025-02-19 17:37</t>
+        </is>
+      </c>
+      <c r="C41" t="n">
+        <v>5</v>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>1,866,309</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>2,304</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>한울소재과학</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>2025-02-19 17:36</t>
+        </is>
+      </c>
+      <c r="C42" t="n">
+        <v>3</v>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>57,502</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>10,869</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix Chrome driver setup and enhance scraping error handling
- Fix Chrome driver initialization to use system ChromeDriver instead of webdriver-manager
- Add explicit Chrome binary path for macOS compatibility
- Add fallback mechanism for ChromeDriverManager if direct approach fails
- Enhance holdings update: automatically read from Excel before refresh operations
- Add smart skip logic: skip companies already up-to-date (last_date = today)
- Improve error handling: save 'unknown' values when table extraction fails but document found
- Update both run_refresh_database and run_all_companies to use latest Excel holdings
- Clean up temporary Excel files and improve logging messages
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20417"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11003"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\kind-refactored\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wonwoolee/Desktop/KINDAPP Project/kind-refactored/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17F7B65E-5B95-4969-9A85-203F99A4ADAA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AE92C48-2743-3F4F-B4F3-7AF30E175506}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="15610" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Holdings" sheetId="1" r:id="rId1"/>
@@ -18,12 +18,12 @@
     <sheet name="PRC_Data" sheetId="3" r:id="rId3"/>
     <sheet name="Summary" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="113">
   <si>
     <t>기업명</t>
   </si>
@@ -37,34 +37,58 @@
     <t>누적_추가주식수</t>
   </si>
   <si>
-    <t>전환가 변동내역</t>
-  </si>
-  <si>
     <t>전환가_변동내역</t>
   </si>
   <si>
+    <t>DB하이텍</t>
+  </si>
+  <si>
+    <t>국도화학</t>
+  </si>
+  <si>
+    <t>녹십자엠에스</t>
+  </si>
+  <si>
+    <t>3,871(2025-05-19 13:50)</t>
+  </si>
+  <si>
+    <t>대원전선</t>
+  </si>
+  <si>
+    <t>드림씨아이에스</t>
+  </si>
+  <si>
     <t>SKAI</t>
   </si>
   <si>
-    <t>7,905(2024-01-08 13:07), 6,900(2024-11-06 14:12), 4,929(2024-11-08 09:57), 4,855(2025-09-22 15:08)</t>
-  </si>
-  <si>
-    <t>미래나노텍</t>
-  </si>
-  <si>
-    <t>켄코아에어로스페이스</t>
-  </si>
-  <si>
-    <t>자화전자</t>
+    <t>7,905(2024-01-08 13:07), 6,900(2024-11-06 14:12), 4,929(2024-11-08 09:57), 4,855(2025-09-22 15:08), 1,458,538(2025-09-22 15:08)</t>
+  </si>
+  <si>
+    <t>삼기에너지솔루션즈</t>
+  </si>
+  <si>
+    <t>삼호개발</t>
   </si>
   <si>
     <t>상아프론테크</t>
   </si>
   <si>
+    <t>서울식품공업</t>
+  </si>
+  <si>
     <t>선익시스템</t>
   </si>
   <si>
-    <t>베뉴지</t>
+    <t>49,591(2025-01-21 11:33)</t>
+  </si>
+  <si>
+    <t>성일하이텍</t>
+  </si>
+  <si>
+    <t>에스엠씨지</t>
+  </si>
+  <si>
+    <t>에스오에스랩</t>
   </si>
   <si>
     <t>에스티팜</t>
@@ -73,16 +97,31 @@
     <t>71,684(2024-02-14 15:55), 79,648(2024-08-09 13:31)</t>
   </si>
   <si>
-    <t>덕우전자</t>
-  </si>
-  <si>
-    <t>8,286(2024-04-01 15:58), 7,985(2024-10-31 17:33)</t>
-  </si>
-  <si>
-    <t>나노신소재</t>
-  </si>
-  <si>
-    <t>117,996(2024-04-22 16:13), 109,198(2024-11-21 15:47)</t>
+    <t>에이럭스</t>
+  </si>
+  <si>
+    <t>이녹스</t>
+  </si>
+  <si>
+    <t>컨텍</t>
+  </si>
+  <si>
+    <t>KH바텍</t>
+  </si>
+  <si>
+    <t>쿠쿠홀딩스</t>
+  </si>
+  <si>
+    <t>테스</t>
+  </si>
+  <si>
+    <t>피아이이</t>
+  </si>
+  <si>
+    <t>한국석유공업</t>
+  </si>
+  <si>
+    <t>흥국에프엔비</t>
   </si>
   <si>
     <t>회사명</t>
@@ -232,6 +271,12 @@
     <t>PRC</t>
   </si>
   <si>
+    <t>KRW : South-Korean Won</t>
+  </si>
+  <si>
+    <t>1,458,538</t>
+  </si>
+  <si>
     <t>2024-11-08 09:57</t>
   </si>
   <si>
@@ -253,40 +298,28 @@
     <t>8,537</t>
   </si>
   <si>
-    <t>2024-11-21 15:47</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>117,996</t>
-  </si>
-  <si>
-    <t>109,198</t>
-  </si>
-  <si>
-    <t>2024-04-22 16:13</t>
-  </si>
-  <si>
-    <t>155,997</t>
-  </si>
-  <si>
-    <t>2024-10-31 17:33</t>
+    <t>2025-05-19 13:50</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>4,043</t>
+  </si>
+  <si>
+    <t>3,871</t>
+  </si>
+  <si>
+    <t>2025-01-21 11:33</t>
   </si>
   <si>
     <t>1</t>
   </si>
   <si>
-    <t>8,286</t>
-  </si>
-  <si>
-    <t>7,985</t>
-  </si>
-  <si>
-    <t>2024-04-01 15:58</t>
-  </si>
-  <si>
-    <t>9,393</t>
+    <t>61,988</t>
+  </si>
+  <si>
+    <t>49,591</t>
   </si>
   <si>
     <t>2024-08-09 13:31</t>
@@ -322,40 +355,32 @@
     <t>생성 시간</t>
   </si>
   <si>
-    <t>2025-10-12 18:11:31</t>
+    <t>2025-10-12 22:34:21</t>
   </si>
   <si>
     <t>데이터베이스 파일 경로</t>
   </si>
   <si>
-    <t>HIST: c:\Users\ASUS\Desktop\kind-refactored\resources\database_hist.json, PRC: c:\Users\ASUS\Desktop\kind-refactored\resources\database_prc.json</t>
+    <t>HIST: /Users/wonwoolee/Desktop/KINDAPP Project/kind-refactored/resources/database_hist.json, PRC: /Users/wonwoolee/Desktop/KINDAPP Project/kind-refactored/resources/database_prc.json</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <name val="맑은 고딕"/>
-      <family val="3"/>
-      <charset val="129"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="맑은 고딕"/>
-      <family val="3"/>
-      <charset val="129"/>
-      <scheme val="minor"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -400,7 +425,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="표준" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -700,15 +725,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="150" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="116.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -724,103 +755,103 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
+      <c r="B2">
+        <v>121</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B2">
-        <v>2</v>
-      </c>
-      <c r="C2">
-        <v>1525491408</v>
-      </c>
-      <c r="D2">
-        <v>313114</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="B3">
+        <v>60</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
+      <c r="B4">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4" t="s">
         <v>8</v>
       </c>
-      <c r="B3">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>9</v>
       </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4">
-        <v>9</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
+      <c r="B5">
+        <v>26</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>10</v>
       </c>
-      <c r="B5">
-        <v>5</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>11</v>
-      </c>
-      <c r="B6">
-        <v>6</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
-        <v>12</v>
       </c>
       <c r="B7">
         <v>2</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>1525491408</v>
       </c>
       <c r="D7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+        <v>313114</v>
+      </c>
+      <c r="E7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>13</v>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -829,59 +860,265 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>14</v>
       </c>
       <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10">
+        <v>6</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11">
+        <v>23</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13">
         <v>2</v>
       </c>
-      <c r="C9">
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17">
         <v>40324030144</v>
       </c>
-      <c r="D9">
+      <c r="D17">
         <v>506278</v>
       </c>
-      <c r="F9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10">
+      <c r="E17" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18">
         <v>1</v>
       </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="F10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11">
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19">
         <v>4</v>
       </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="F11" t="s">
-        <v>19</v>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21">
+        <v>4</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23">
+        <v>2</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>31</v>
+      </c>
+      <c r="B25">
+        <v>2</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>32</v>
+      </c>
+      <c r="B26">
+        <v>4</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -890,25 +1127,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="106" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="7" max="7" width="48.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>3</v>
@@ -917,24 +1159,24 @@
         <v>2</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="D2" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="E2" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="F2">
         <v>313114</v>
@@ -943,24 +1185,24 @@
         <v>1525491408</v>
       </c>
       <c r="H2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="D3" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="E3" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="F3">
         <v>125245</v>
@@ -969,24 +1211,24 @@
         <v>610193640</v>
       </c>
       <c r="H3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="C4" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="D4" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="E4" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="F4">
         <v>31311</v>
@@ -995,24 +1237,24 @@
         <v>152547192</v>
       </c>
       <c r="H4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="C5" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="D5" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="E5" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="F5">
         <v>506278</v>
@@ -1021,24 +1263,24 @@
         <v>40324030144</v>
       </c>
       <c r="H5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="C6" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="D6" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="E6" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="F6">
         <v>471122</v>
@@ -1047,24 +1289,24 @@
         <v>37523925056</v>
       </c>
       <c r="H6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B7" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="C7" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="D7" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="E7" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="F7">
         <v>453544</v>
@@ -1073,24 +1315,24 @@
         <v>36123872512</v>
       </c>
       <c r="H7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="C8" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="D8" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="E8" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="F8">
         <v>449778</v>
@@ -1099,24 +1341,24 @@
         <v>35823918144</v>
       </c>
       <c r="H8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B9" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="D9" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="E9" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="F9">
         <v>444756</v>
@@ -1125,24 +1367,24 @@
         <v>35423925888</v>
       </c>
       <c r="H9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B10" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="D10" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="E10" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="F10">
         <v>425924</v>
@@ -1151,24 +1393,24 @@
         <v>33923994752</v>
       </c>
       <c r="H10" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B11" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="C11" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="D11" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="E11" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="F11">
         <v>403953</v>
@@ -1177,24 +1419,24 @@
         <v>32174048544</v>
       </c>
       <c r="H11" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" t="s">
+        <v>63</v>
+      </c>
+      <c r="E12" t="s">
         <v>49</v>
-      </c>
-      <c r="C12" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" t="s">
-        <v>50</v>
-      </c>
-      <c r="E12" t="s">
-        <v>36</v>
       </c>
       <c r="F12">
         <v>381354</v>
@@ -1203,24 +1445,24 @@
         <v>30374083392</v>
       </c>
       <c r="H12" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B13" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" t="s">
+        <v>59</v>
+      </c>
+      <c r="E13" t="s">
         <v>49</v>
-      </c>
-      <c r="C13" t="s">
-        <v>26</v>
-      </c>
-      <c r="D13" t="s">
-        <v>46</v>
-      </c>
-      <c r="E13" t="s">
-        <v>36</v>
       </c>
       <c r="F13">
         <v>338039</v>
@@ -1229,24 +1471,24 @@
         <v>26924130272</v>
       </c>
       <c r="H13" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B14" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="C14" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="D14" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="E14" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="F14">
         <v>316068</v>
@@ -1255,24 +1497,24 @@
         <v>25174184064</v>
       </c>
       <c r="H14" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B15" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
       <c r="C15" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="D15" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="E15" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="F15">
         <v>149087</v>
@@ -1281,24 +1523,24 @@
         <v>11874481376</v>
       </c>
       <c r="H15" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B16" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
       <c r="C16" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="D16" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
       <c r="E16" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="F16">
         <v>196796</v>
@@ -1307,24 +1549,24 @@
         <v>15674407808</v>
       </c>
       <c r="H16" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B17" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="C17" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="D17" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="E17" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="F17">
         <v>131510</v>
@@ -1333,24 +1575,24 @@
         <v>10474508480</v>
       </c>
       <c r="H17" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B18" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="C18" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="D18" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="E18" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="F18">
         <v>98871</v>
@@ -1359,24 +1601,24 @@
         <v>7874877408</v>
       </c>
       <c r="H18" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B19" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
       <c r="C19" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="D19" t="s">
-        <v>61</v>
+        <v>74</v>
       </c>
       <c r="E19" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="F19">
         <v>48337</v>
@@ -1385,24 +1627,24 @@
         <v>3849945376</v>
       </c>
       <c r="H19" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B20" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="C20" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="D20" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="E20" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="F20">
         <v>43943</v>
@@ -1411,245 +1653,225 @@
         <v>3499972064</v>
       </c>
       <c r="H20" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="167" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>65</v>
+        <v>78</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="D2" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="E2" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="F2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="D3" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="E3" t="s">
-        <v>71</v>
+        <v>83</v>
       </c>
       <c r="F3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>72</v>
+        <v>84</v>
       </c>
       <c r="C4" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="D4" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
       <c r="E4" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="F4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
       <c r="C5" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="D5" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
       <c r="E5" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
       <c r="F5" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>76</v>
+        <v>89</v>
       </c>
       <c r="C6" t="s">
-        <v>77</v>
+        <v>39</v>
       </c>
       <c r="D6" t="s">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="E6" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="F6" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="C7" t="s">
-        <v>77</v>
+        <v>92</v>
       </c>
       <c r="D7" t="s">
+        <v>93</v>
+      </c>
+      <c r="E7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F7" t="s">
         <v>81</v>
       </c>
-      <c r="E7" t="s">
-        <v>78</v>
-      </c>
-      <c r="F7" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>82</v>
+        <v>95</v>
       </c>
       <c r="C8" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
       <c r="D8" t="s">
-        <v>84</v>
+        <v>97</v>
       </c>
       <c r="E8" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
       <c r="F8" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B9" t="s">
-        <v>86</v>
+        <v>99</v>
       </c>
       <c r="C9" t="s">
-        <v>83</v>
+        <v>39</v>
       </c>
       <c r="D9" t="s">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="E9" t="s">
-        <v>84</v>
+        <v>49</v>
       </c>
       <c r="F9" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B10" t="s">
-        <v>88</v>
+        <v>101</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="D10" t="s">
-        <v>89</v>
+        <v>49</v>
       </c>
       <c r="E10" t="s">
-        <v>36</v>
+        <v>100</v>
       </c>
       <c r="F10" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" t="s">
-        <v>90</v>
-      </c>
-      <c r="C11" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" t="s">
-        <v>36</v>
-      </c>
-      <c r="E11" t="s">
-        <v>89</v>
-      </c>
-      <c r="F11" t="s">
-        <v>68</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -1660,66 +1882,65 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="B2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="B3">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>95</v>
+        <v>106</v>
       </c>
       <c r="B4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>96</v>
+        <v>107</v>
       </c>
       <c r="B5" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>98</v>
+        <v>109</v>
       </c>
       <c r="B6" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>100</v>
+        <v>111</v>
       </c>
       <c r="B7" t="s">
-        <v>101</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>